<commit_message>
(EN PROCESO) Implementacion XLS para Seguimiento Pycks
</commit_message>
<xml_diff>
--- a/Requerimientos/Diseño_GananciasPerdidas.xlsx
+++ b/Requerimientos/Diseño_GananciasPerdidas.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\git\UBet\Requerimientos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -63,6 +58,9 @@
   </si>
   <si>
     <t>Win</t>
+  </si>
+  <si>
+    <t>TotalPycks</t>
   </si>
 </sst>
 </file>
@@ -106,6 +104,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -125,7 +191,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="E0DFE3"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -372,7 +438,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -383,7 +449,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,6 +472,9 @@
       <c r="C1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">

</xml_diff>